<commit_message>
data and script update
update latest data file and new script. New figures available in figure/new
</commit_message>
<xml_diff>
--- a/analysis/SubIDs_new.xlsx
+++ b/analysis/SubIDs_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGABYTE\AppData\LocalLow\Rokers Vision Lab\Vision VR\Ben-s-capstone-data-analysis\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD27FFC-1333-4F4F-84EC-2CD77983A19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB8264E-5798-463D-A578-457B657BB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="session 1" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -207,11 +207,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -265,6 +276,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,8 +506,8 @@
   </sheetPr>
   <dimension ref="A1:K988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -712,17 +732,75 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="G8" s="4"/>
+    <row r="8" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6">
+        <v>59.5</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.98</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.94</v>
+      </c>
+      <c r="G8" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1.65</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="K8" s="5">
+        <v>1.8</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="A9" s="22">
+        <v>15</v>
+      </c>
+      <c r="B9" s="23">
+        <v>62.5</v>
+      </c>
+      <c r="C9" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="D9" s="22">
+        <v>0.62</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0.06</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0.74</v>
+      </c>
+      <c r="G9" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="H9" s="22">
+        <v>0.66</v>
+      </c>
+      <c r="I9" s="22">
+        <v>1.85</v>
+      </c>
+      <c r="J9" s="22">
+        <v>1.85</v>
+      </c>
+      <c r="K9" s="22">
+        <v>1.9</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -6615,10 +6693,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3384E2-A090-4B09-AB7D-D221A28F9F0C}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6682,7 +6760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
       <c r="B3" s="17"/>
       <c r="C3" s="12" t="s">
@@ -6721,25 +6799,25 @@
         <v>65.5</v>
       </c>
       <c r="C4" s="7">
+        <v>-0.16</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.62</v>
+      </c>
+      <c r="E4" s="7">
+        <v>-0.1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="G4" s="7">
         <v>-0.18</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="G4" s="7">
-        <v>-0.1</v>
       </c>
       <c r="H4" s="5">
         <v>0.4</v>
       </c>
       <c r="I4" s="5">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="J4" s="5">
         <v>1.65</v>
@@ -6756,19 +6834,19 @@
         <v>67.5</v>
       </c>
       <c r="C5" s="7">
-        <v>0.1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D5" s="5">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="E5" s="7">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="F5" s="5">
         <v>1.1000000000000001</v>
       </c>
       <c r="G5" s="7">
-        <v>-0.08</v>
+        <v>0</v>
       </c>
       <c r="H5" s="5">
         <v>0.98</v>
@@ -6777,10 +6855,10 @@
         <v>1.65</v>
       </c>
       <c r="J5" s="5">
-        <v>1.65</v>
+        <v>1.8</v>
       </c>
       <c r="K5" s="5">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -6791,13 +6869,13 @@
         <v>64</v>
       </c>
       <c r="C6" s="7">
-        <v>-0.06</v>
+        <v>-0.02</v>
       </c>
       <c r="D6" s="5">
         <v>1.1000000000000001</v>
       </c>
       <c r="E6" s="7">
-        <v>0.02</v>
+        <v>-0.02</v>
       </c>
       <c r="F6" s="5">
         <v>1.1000000000000001</v>
@@ -6826,31 +6904,101 @@
         <v>63.5</v>
       </c>
       <c r="C7" s="7">
-        <v>-0.04</v>
+        <v>0</v>
       </c>
       <c r="D7" s="5">
-        <v>1.06</v>
+        <v>0.82</v>
       </c>
       <c r="E7" s="7">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="F7" s="5">
-        <v>1</v>
+        <v>0.76</v>
       </c>
       <c r="G7" s="7">
         <v>-0.1</v>
       </c>
       <c r="H7" s="5">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="I7" s="5">
         <v>1.65</v>
       </c>
       <c r="J7" s="5">
-        <v>1.65</v>
+        <v>1.8</v>
       </c>
       <c r="K7" s="5">
         <v>1.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6">
+        <v>59.5</v>
+      </c>
+      <c r="C8" s="7">
+        <v>-0.06</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.94</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>-0.06</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1.65</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="K8" s="5">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>15</v>
+      </c>
+      <c r="B9" s="23">
+        <v>62.5</v>
+      </c>
+      <c r="C9" s="24">
+        <v>-0.04</v>
+      </c>
+      <c r="D9" s="22">
+        <v>0.68</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0.66</v>
+      </c>
+      <c r="G9" s="24">
+        <v>0</v>
+      </c>
+      <c r="H9" s="22">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I9" s="22">
+        <v>1.85</v>
+      </c>
+      <c r="J9" s="22">
+        <v>1.85</v>
+      </c>
+      <c r="K9" s="22">
+        <v>1.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>